<commit_message>
no Q7, done Q8 pt1
</commit_message>
<xml_diff>
--- a/spreadsheets/metro_budget_exercise.xlsx
+++ b/spreadsheets/metro_budget_exercise.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkwhi\Documents\nss_data_analytics\Projects\lookups-budget-t-white-21\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6F106B-B40F-4FCF-B15D-8E5C102369EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFE0B0A-73D9-4FD9-8D00-4A41BD2380D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="80" windowWidth="21720" windowHeight="13780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
     <sheet name="data_dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metro_budget!$A$1:$P$52</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="92">
   <si>
     <t>Department</t>
   </si>
@@ -307,6 +310,9 @@
   </si>
   <si>
     <t>7. Modify your formulas from questions 3-5 using MATCH so that you can pull the formula both down and sideways to fill in the entire table.</t>
+  </si>
+  <si>
+    <t>8. Use XLOOKUP to find, for each financial year, the three highest ranked departments in terms of the percentage below budget their actual spending was. Bonus: Combine XLOOKUP with INDEX and MATCH in order to write two formulas that can be copied and pasted to fill in the table.</t>
   </si>
 </sst>
 </file>
@@ -773,7 +779,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -816,8 +822,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -835,8 +842,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -876,6 +894,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -1190,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P100"/>
+  <dimension ref="A1:P105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1201,7 +1220,7 @@
     <col min="1" max="1" width="32.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="26.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.81640625" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.54296875" customWidth="1"/>
     <col min="8" max="8" width="26.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="15.81640625" customWidth="1"/>
@@ -1226,7 +1245,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -1278,9 +1297,9 @@
         <f>IFERROR(D2/B2,"")</f>
         <v>-4.3170750765267295E-2</v>
       </c>
-      <c r="F2">
-        <f>IFERROR(RANK(E2,E:E),"")</f>
-        <v>36</v>
+      <c r="F2" s="17">
+        <f>IFERROR(RANK(E2,$E$2:$E$52),"")</f>
+        <v>35</v>
       </c>
       <c r="G2">
         <v>382685200</v>
@@ -1337,9 +1356,9 @@
         <f t="shared" ref="E3:E52" si="1">IFERROR(D3/B3,"")</f>
         <v>-2.3069981751824741E-2</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F10" si="2">IFERROR(RANK(E3,E:E),"")</f>
-        <v>28</v>
+      <c r="F3" s="17">
+        <f t="shared" ref="F3:F52" si="2">IFERROR(RANK(E3,$E$2:$E$52),"")</f>
+        <v>27</v>
       </c>
       <c r="G3">
         <v>334800</v>
@@ -1396,9 +1415,9 @@
         <f t="shared" si="1"/>
         <v>-4.9327413275443007E-3</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="17">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4">
         <v>3652300</v>
@@ -1455,9 +1474,9 @@
         <f t="shared" si="1"/>
         <v>-9.4273968477453174E-2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="17">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5">
         <v>7968300</v>
@@ -1514,9 +1533,9 @@
         <f t="shared" si="1"/>
         <v>-5.7149963352064452E-2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="17">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -1573,9 +1592,9 @@
         <f t="shared" si="1"/>
         <v>-0.11502817362571344</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="17">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7">
         <v>3390900</v>
@@ -1632,9 +1651,9 @@
         <f t="shared" si="1"/>
         <v>-0.15235918433091292</v>
       </c>
-      <c r="F8">
-        <f>IFERROR(RANK(E8,E:E),"")</f>
-        <v>49</v>
+      <c r="F8" s="17">
+        <f t="shared" si="2"/>
+        <v>48</v>
       </c>
       <c r="G8">
         <v>1590700</v>
@@ -1691,9 +1710,9 @@
         <f t="shared" si="1"/>
         <v>-4.2417130511048909E-2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="17">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -1750,9 +1769,9 @@
         <f t="shared" si="1"/>
         <v>-8.1681998646514792E-2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="17">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -1809,8 +1828,8 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F11" t="str">
-        <f t="shared" ref="F3:F52" si="9">IFERROR(_xlfn.RANK.AVG(E11,E:E),"")</f>
+      <c r="F11" s="17" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G11">
@@ -1868,9 +1887,9 @@
         <f t="shared" si="1"/>
         <v>-5.0060657805601608E-2</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="9"/>
-        <v>37</v>
+      <c r="F12" s="17">
+        <f t="shared" si="2"/>
+        <v>36</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -1927,9 +1946,9 @@
         <f t="shared" si="1"/>
         <v>-1.2912833886247806E-2</v>
       </c>
-      <c r="F13">
-        <f>IFERROR(_xlfn.RANK.AVG(E13,E:E),"")</f>
-        <v>17</v>
+      <c r="F13" s="17">
+        <f t="shared" si="2"/>
+        <v>16</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -1986,9 +2005,9 @@
         <f t="shared" si="1"/>
         <v>-1.3637949218750009E-2</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="9"/>
-        <v>20</v>
+      <c r="F14" s="17">
+        <f t="shared" si="2"/>
+        <v>19</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -2045,9 +2064,9 @@
         <f t="shared" si="1"/>
         <v>3.1837408866824991E-3</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="9"/>
-        <v>2</v>
+      <c r="F15" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>184167800</v>
@@ -2104,9 +2123,9 @@
         <f t="shared" si="1"/>
         <v>-1.1850188616360429E-2</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="9"/>
-        <v>13</v>
+      <c r="F16" s="17">
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -2163,9 +2182,9 @@
         <f t="shared" si="1"/>
         <v>-2.8351094826658003E-2</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="9"/>
-        <v>29</v>
+      <c r="F17" s="17">
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -2222,9 +2241,9 @@
         <f t="shared" si="1"/>
         <v>-5.4037002206391245E-2</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="9"/>
-        <v>38</v>
+      <c r="F18" s="17">
+        <f t="shared" si="2"/>
+        <v>37</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -2281,9 +2300,9 @@
         <f t="shared" si="1"/>
         <v>-4.258504294298146E-2</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="9"/>
-        <v>35</v>
+      <c r="F19" s="17">
+        <f t="shared" si="2"/>
+        <v>34</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -2340,9 +2359,9 @@
         <f t="shared" si="1"/>
         <v>-1.2379538203300809E-5</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="9"/>
-        <v>4</v>
+      <c r="F20" s="17">
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -2399,9 +2418,9 @@
         <f t="shared" si="1"/>
         <v>-7.9052463618023094E-2</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="9"/>
-        <v>41</v>
+      <c r="F21" s="17">
+        <f t="shared" si="2"/>
+        <v>40</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -2458,9 +2477,9 @@
         <f t="shared" si="1"/>
         <v>-1.3285502334437123E-2</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="9"/>
-        <v>18</v>
+      <c r="F22" s="17">
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -2517,9 +2536,9 @@
         <f t="shared" si="1"/>
         <v>-3.9590110100806722E-2</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="9"/>
-        <v>32</v>
+      <c r="F23" s="17">
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -2576,9 +2595,9 @@
         <f t="shared" si="1"/>
         <v>-1.3334943305713101E-2</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="9"/>
-        <v>19</v>
+      <c r="F24" s="17">
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -2635,9 +2654,9 @@
         <f t="shared" si="1"/>
         <v>-1.0226130964676661E-2</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="9"/>
-        <v>12</v>
+      <c r="F25" s="17">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -2694,9 +2713,9 @@
         <f t="shared" si="1"/>
         <v>-8.5306091660634673E-2</v>
       </c>
-      <c r="F26">
-        <f t="shared" si="9"/>
-        <v>45</v>
+      <c r="F26" s="17">
+        <f t="shared" si="2"/>
+        <v>44</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -2753,8 +2772,8 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F27" t="str">
-        <f t="shared" si="9"/>
+      <c r="F27" s="17" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G27">
@@ -2812,9 +2831,9 @@
         <f t="shared" si="1"/>
         <v>-9.5782760864849215E-2</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="9"/>
-        <v>47</v>
+      <c r="F28" s="17">
+        <f t="shared" si="2"/>
+        <v>46</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -2871,9 +2890,9 @@
         <f t="shared" si="1"/>
         <v>-1.4800253727847622E-2</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="9"/>
-        <v>22</v>
+      <c r="F29" s="17">
+        <f t="shared" si="2"/>
+        <v>21</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -2930,9 +2949,9 @@
         <f t="shared" si="1"/>
         <v>-8.3831374359143746E-3</v>
       </c>
-      <c r="F30">
-        <f t="shared" si="9"/>
-        <v>10</v>
+      <c r="F30" s="17">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -2989,9 +3008,9 @@
         <f t="shared" si="1"/>
         <v>-1.4030533529678329E-2</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="9"/>
-        <v>21</v>
+      <c r="F31" s="17">
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -3048,9 +3067,9 @@
         <f t="shared" si="1"/>
         <v>-1.2294942827617691E-2</v>
       </c>
-      <c r="F32">
-        <f t="shared" si="9"/>
-        <v>14</v>
+      <c r="F32" s="17">
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -3107,9 +3126,9 @@
         <f t="shared" si="1"/>
         <v>-7.9969930789269058E-3</v>
       </c>
-      <c r="F33">
-        <f t="shared" si="9"/>
-        <v>9</v>
+      <c r="F33" s="17">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -3166,9 +3185,9 @@
         <f t="shared" si="1"/>
         <v>-1.8939149738619768E-2</v>
       </c>
-      <c r="F34">
-        <f t="shared" si="9"/>
-        <v>24</v>
+      <c r="F34" s="17">
+        <f t="shared" si="2"/>
+        <v>23</v>
       </c>
       <c r="G34">
         <v>4350600</v>
@@ -3225,8 +3244,8 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F35" t="str">
-        <f t="shared" si="9"/>
+      <c r="F35" s="17" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G35">
@@ -3284,9 +3303,9 @@
         <f t="shared" si="1"/>
         <v>-7.8647857679780775E-2</v>
       </c>
-      <c r="F36">
-        <f t="shared" si="9"/>
-        <v>40</v>
+      <c r="F36" s="17">
+        <f t="shared" si="2"/>
+        <v>39</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -3343,9 +3362,9 @@
         <f t="shared" si="1"/>
         <v>-3.9444515758219188E-2</v>
       </c>
-      <c r="F37">
-        <f t="shared" si="9"/>
-        <v>31</v>
+      <c r="F37" s="17">
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -3402,9 +3421,9 @@
         <f t="shared" si="1"/>
         <v>-1.9443680579913542E-2</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="9"/>
-        <v>25</v>
+      <c r="F38" s="17">
+        <f t="shared" si="2"/>
+        <v>24</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -3461,9 +3480,9 @@
         <f t="shared" si="1"/>
         <v>-8.008952370177623E-2</v>
       </c>
-      <c r="F39">
-        <f t="shared" si="9"/>
-        <v>42</v>
+      <c r="F39" s="17">
+        <f t="shared" si="2"/>
+        <v>41</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -3520,9 +3539,9 @@
         <f t="shared" si="1"/>
         <v>-2.1279773539092578E-2</v>
       </c>
-      <c r="F40">
-        <f t="shared" si="9"/>
-        <v>27</v>
+      <c r="F40" s="17">
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -3579,9 +3598,9 @@
         <f t="shared" si="1"/>
         <v>-4.0110550149132493E-2</v>
       </c>
-      <c r="F41">
-        <f t="shared" si="9"/>
-        <v>33</v>
+      <c r="F41" s="17">
+        <f t="shared" si="2"/>
+        <v>32</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -3638,9 +3657,9 @@
         <f t="shared" si="1"/>
         <v>-2.2070943135841053E-4</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="9"/>
-        <v>6</v>
+      <c r="F42" s="17">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -3697,9 +3716,9 @@
         <f t="shared" si="1"/>
         <v>-2.0497353541313264E-2</v>
       </c>
-      <c r="F43">
-        <f t="shared" si="9"/>
-        <v>26</v>
+      <c r="F43" s="17">
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -3756,9 +3775,9 @@
         <f t="shared" si="1"/>
         <v>-9.7760750186150751E-3</v>
       </c>
-      <c r="F44">
-        <f t="shared" si="9"/>
-        <v>11</v>
+      <c r="F44" s="17">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -3815,9 +3834,9 @@
         <f t="shared" si="1"/>
         <v>-1.287514194887851E-2</v>
       </c>
-      <c r="F45">
-        <f t="shared" si="9"/>
-        <v>16</v>
+      <c r="F45" s="17">
+        <f t="shared" si="2"/>
+        <v>15</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -3874,9 +3893,9 @@
         <f t="shared" si="1"/>
         <v>-3.0010420686993711E-3</v>
       </c>
-      <c r="F46">
-        <f t="shared" si="9"/>
-        <v>7</v>
+      <c r="F46" s="17">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -3933,9 +3952,9 @@
         <f t="shared" si="1"/>
         <v>-1.7435939690898361E-4</v>
       </c>
-      <c r="F47">
-        <f t="shared" si="9"/>
-        <v>5</v>
+      <c r="F47" s="17">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -3992,9 +4011,9 @@
         <f t="shared" si="1"/>
         <v>-3.1133192323107857E-2</v>
       </c>
-      <c r="F48">
-        <f t="shared" si="9"/>
-        <v>30</v>
+      <c r="F48" s="17">
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -4051,9 +4070,9 @@
         <f t="shared" si="1"/>
         <v>-1.8444360086767971E-2</v>
       </c>
-      <c r="F49">
-        <f t="shared" si="9"/>
-        <v>23</v>
+      <c r="F49" s="17">
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -4110,9 +4129,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F50">
-        <f t="shared" si="9"/>
-        <v>3</v>
+      <c r="F50" s="17">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -4169,9 +4188,9 @@
         <f t="shared" si="1"/>
         <v>-1.2785255822058129E-2</v>
       </c>
-      <c r="F51">
-        <f t="shared" si="9"/>
-        <v>15</v>
+      <c r="F51" s="17">
+        <f t="shared" si="2"/>
+        <v>14</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -4228,9 +4247,9 @@
         <f t="shared" si="1"/>
         <v>-8.009596083231342E-2</v>
       </c>
-      <c r="F52">
-        <f t="shared" si="9"/>
-        <v>43</v>
+      <c r="F52" s="17">
+        <f t="shared" si="2"/>
+        <v>42</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -4290,6 +4309,18 @@
       <c r="E55" s="9" t="s">
         <v>90</v>
       </c>
+      <c r="F55" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56" spans="1:16">
       <c r="A56" t="s">
@@ -4308,6 +4339,21 @@
         <v>-9181.0800000000163</v>
       </c>
       <c r="E56" s="10"/>
+      <c r="F56" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56">
+        <f>INDEX(D$2:D$52,MATCH($F56,$A$2:$A$52))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="H56">
+        <f t="shared" ref="H56:I61" si="9">INDEX(E$2:E$52,MATCH($F56,$A$2:$A$52))</f>
+        <v>-8.1681998646514792E-2</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="9"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="57" spans="1:16">
       <c r="A57" t="s">
@@ -4326,6 +4372,21 @@
         <v>-311228.08999999997</v>
       </c>
       <c r="E57" s="10"/>
+      <c r="F57" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57">
+        <f t="shared" ref="G57:G61" si="12">INDEX(D$2:D$52,MATCH($F57,$A$2:$A$52))</f>
+        <v>0</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
     </row>
     <row r="58" spans="1:16">
       <c r="A58" t="s">
@@ -4344,6 +4405,21 @@
         <v>-374962.91000000015</v>
       </c>
       <c r="E58" s="10"/>
+      <c r="F58" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="12"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="9"/>
+        <v>-5.4037002206391245E-2</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="9"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="59" spans="1:16">
       <c r="A59" t="s">
@@ -4362,6 +4438,21 @@
         <v>-72.879999999888241</v>
       </c>
       <c r="E59" s="10"/>
+      <c r="F59" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="12"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="9"/>
+        <v>-1.3334943305713101E-2</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="9"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="60" spans="1:16">
       <c r="A60" t="s">
@@ -4380,6 +4471,21 @@
         <v>-1724.9000000000233</v>
       </c>
       <c r="E60" s="10"/>
+      <c r="F60" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="12"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="9"/>
+        <v>-1.0226130964676661E-2</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="61" spans="1:16">
       <c r="A61" t="s">
@@ -4398,6 +4504,21 @@
         <v>-82077.349999999627</v>
       </c>
       <c r="E61" s="10"/>
+      <c r="F61" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="12"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="9"/>
+        <v>-4.0110550149132493E-2</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="9"/>
+        <v>32</v>
+      </c>
     </row>
     <row r="62" spans="1:16">
       <c r="E62" s="10"/>
@@ -4443,15 +4564,15 @@
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="12">_xlfn.XLOOKUP(A66,A$1:A$52,D$1:D$52)</f>
+        <f t="shared" ref="B66:B70" si="13">_xlfn.XLOOKUP(A66,A$1:A$52,D$1:D$52)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="13">_xlfn.XLOOKUP($A66,$A$1:$A$52,I$1:I$52)</f>
+        <f t="shared" ref="C66:C70" si="14">_xlfn.XLOOKUP($A66,$A$1:$A$52,I$1:I$52)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP($A66,$A$1:$A$52,N$1:N$52)</f>
+        <f t="shared" ref="D66:D70" si="15">_xlfn.XLOOKUP($A66,$A$1:$A$52,N$1:N$52)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4460,15 +4581,15 @@
         <v>32</v>
       </c>
       <c r="B67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4477,15 +4598,15 @@
         <v>38</v>
       </c>
       <c r="B68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4494,15 +4615,15 @@
         <v>39</v>
       </c>
       <c r="B69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4511,15 +4632,15 @@
         <v>55</v>
       </c>
       <c r="B70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4568,11 +4689,11 @@
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="15">INDEX(I$1:I$52,MATCH($A75,$A$1:$A$52))</f>
+        <f t="shared" ref="C75:C79" si="16">INDEX(I$1:I$52,MATCH($A75,$A$1:$A$52))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="16">INDEX(N$1:N$52,MATCH($A75,$A$1:$A$52))</f>
+        <f t="shared" ref="D75:D79" si="17">INDEX(N$1:N$52,MATCH($A75,$A$1:$A$52))</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4585,11 +4706,11 @@
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4602,11 +4723,11 @@
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4619,11 +4740,11 @@
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4636,11 +4757,11 @@
         <v>-184239.79000001028</v>
       </c>
       <c r="C79">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4726,7 +4847,7 @@
         <v>2</v>
       </c>
       <c r="E89" s="7"/>
-      <c r="F89" s="7">
+      <c r="F89" s="15">
         <v>3</v>
       </c>
     </row>
@@ -4743,7 +4864,7 @@
       <c r="E90" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F90" s="8" t="s">
+      <c r="F90" s="16" t="s">
         <v>0</v>
       </c>
       <c r="G90" s="8" t="s">
@@ -4754,25 +4875,88 @@
       <c r="A91" t="s">
         <v>73</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="G91" s="5"/>
+      <c r="B91" t="str">
+        <f>_xlfn.XLOOKUP(B$89,$F$1:$F$52,$A$1:$A$52)</f>
+        <v>Debt Service</v>
+      </c>
+      <c r="C91" s="12">
+        <f>_xlfn.XLOOKUP(B91,$A$1:$A$52,$E$1:$E$52)</f>
+        <v>3.1837408866824991E-3</v>
+      </c>
+      <c r="D91" t="str">
+        <f>_xlfn.XLOOKUP(D$89,$F$1:$F$52,$A$1:$A$52)</f>
+        <v>Sports Authority</v>
+      </c>
+      <c r="E91" s="12">
+        <f>_xlfn.XLOOKUP(D91,$A$1:$A$52,$E$1:$E$52)</f>
+        <v>0</v>
+      </c>
+      <c r="F91" s="13" t="str">
+        <f>_xlfn.XLOOKUP(F$89,$F$1:$F$52,$A$1:$A$52)</f>
+        <v>Fire</v>
+      </c>
+      <c r="G91" s="12">
+        <f>_xlfn.XLOOKUP(F91,$A$1:$A$52,$E$1:$E$52)</f>
+        <v>-1.2379538203300809E-5</v>
+      </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="G92" s="5"/>
+      <c r="B92" t="str">
+        <f>_xlfn.XLOOKUP(B$89,$K$1:$K$52,$A$1:$A$52)</f>
+        <v>Sports Authority</v>
+      </c>
+      <c r="C92" s="12">
+        <f>_xlfn.XLOOKUP(B92,$A$1:$A$52,$J$1:$J$52)</f>
+        <v>0</v>
+      </c>
+      <c r="D92" t="str">
+        <f>_xlfn.XLOOKUP(D$89,$K$1:$K$52,$A$1:$A$52)</f>
+        <v>Fire</v>
+      </c>
+      <c r="E92" s="12">
+        <f>_xlfn.XLOOKUP(D92,$A$1:$A$52,$J$1:$J$52)</f>
+        <v>-7.4142392760188761E-5</v>
+      </c>
+      <c r="F92" s="13" t="str">
+        <f>_xlfn.XLOOKUP(F$89,$K$1:$K$52,$A$1:$A$52)</f>
+        <v>District Attorney</v>
+      </c>
+      <c r="G92" s="12">
+        <f>_xlfn.XLOOKUP(F92,$A$1:$A$52,$J$1:$J$52)</f>
+        <v>-2.769017341040361E-4</v>
+      </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>75</v>
       </c>
-      <c r="C93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="G93" s="5"/>
+      <c r="B93" t="str">
+        <f>_xlfn.XLOOKUP(B$89,$P$1:$P$52,$A$1:$A$52)</f>
+        <v>Sports Authority</v>
+      </c>
+      <c r="C93" s="12">
+        <f>_xlfn.XLOOKUP(B93,$A$1:$A$52,$O$1:$O$52)</f>
+        <v>0</v>
+      </c>
+      <c r="D93" t="str">
+        <f>_xlfn.XLOOKUP(D$89,$P$1:$P$52,$A$1:$A$52)</f>
+        <v>Police</v>
+      </c>
+      <c r="E93" s="12">
+        <f>_xlfn.XLOOKUP(D93,$A$1:$A$52,$O$1:$O$52)</f>
+        <v>-1.8129115815929696E-7</v>
+      </c>
+      <c r="F93" s="13" t="str">
+        <f>_xlfn.XLOOKUP(F$89,$P$1:$P$52,$A$1:$A$52)</f>
+        <v>Fire</v>
+      </c>
+      <c r="G93" s="12">
+        <f>_xlfn.XLOOKUP(F93,$A$1:$A$52,$O$1:$O$52)</f>
+        <v>-8.9158438821450736E-7</v>
+      </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="7" t="s">
@@ -4791,7 +4975,7 @@
         <v>2</v>
       </c>
       <c r="E96" s="7"/>
-      <c r="F96" s="7">
+      <c r="F96" s="15">
         <v>3</v>
       </c>
     </row>
@@ -4808,7 +4992,7 @@
       <c r="E97" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F97" s="8" t="s">
+      <c r="F97" s="16" t="s">
         <v>0</v>
       </c>
       <c r="G97" s="8" t="s">
@@ -4842,18 +5026,37 @@
       <c r="G100" s="4"/>
       <c r="I100" s="4"/>
     </row>
+    <row r="103" spans="1:9">
+      <c r="A103" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B103" s="11"/>
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" s="11"/>
+      <c r="B104" s="11"/>
+      <c r="C104" s="11"/>
+      <c r="D104" s="11"/>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="11"/>
+      <c r="B105" s="11"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <autoFilter ref="A1:P52" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <mergeCells count="2">
     <mergeCell ref="E55:E62"/>
+    <mergeCell ref="A103:D105"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A82:A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A82" xr:uid="{EBC7F037-5A59-4B81-92DB-547E5D4B4917}">
-      <formula1>$A$2:$A$52</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
done Q9, stumped on Q7
</commit_message>
<xml_diff>
--- a/spreadsheets/metro_budget_exercise.xlsx
+++ b/spreadsheets/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkwhi\Documents\nss_data_analytics\Projects\lookups-budget-t-white-21\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFE0B0A-73D9-4FD9-8D00-4A41BD2380D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227FEA6D-C4AF-4A3D-86A0-51BE247231BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="80" windowWidth="21720" windowHeight="13780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="93">
   <si>
     <t>Department</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>8. Use XLOOKUP to find, for each financial year, the three highest ranked departments in terms of the percentage below budget their actual spending was. Bonus: Combine XLOOKUP with INDEX and MATCH in order to write two formulas that can be copied and pasted to fill in the table.</t>
+  </si>
+  <si>
+    <t>9. Do the same as above, but using only INDEX and MATCH.</t>
   </si>
 </sst>
 </file>
@@ -824,7 +827,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -836,6 +839,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -843,16 +847,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1209,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P105"/>
+  <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1297,7 +1301,7 @@
         <f>IFERROR(D2/B2,"")</f>
         <v>-4.3170750765267295E-2</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="13">
         <f>IFERROR(RANK(E2,$E$2:$E$52),"")</f>
         <v>35</v>
       </c>
@@ -1356,7 +1360,7 @@
         <f t="shared" ref="E3:E52" si="1">IFERROR(D3/B3,"")</f>
         <v>-2.3069981751824741E-2</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="13">
         <f t="shared" ref="F3:F52" si="2">IFERROR(RANK(E3,$E$2:$E$52),"")</f>
         <v>27</v>
       </c>
@@ -1415,7 +1419,7 @@
         <f t="shared" si="1"/>
         <v>-4.9327413275443007E-3</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="13">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
@@ -1474,7 +1478,7 @@
         <f t="shared" si="1"/>
         <v>-9.4273968477453174E-2</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="13">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
@@ -1533,7 +1537,7 @@
         <f t="shared" si="1"/>
         <v>-5.7149963352064452E-2</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="13">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
@@ -1592,7 +1596,7 @@
         <f t="shared" si="1"/>
         <v>-0.11502817362571344</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="13">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
@@ -1651,7 +1655,7 @@
         <f t="shared" si="1"/>
         <v>-0.15235918433091292</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="13">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
@@ -1710,7 +1714,7 @@
         <f t="shared" si="1"/>
         <v>-4.2417130511048909E-2</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="13">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
@@ -1769,7 +1773,7 @@
         <f t="shared" si="1"/>
         <v>-8.1681998646514792E-2</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
@@ -1828,7 +1832,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F11" s="17" t="str">
+      <c r="F11" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1887,7 +1891,7 @@
         <f t="shared" si="1"/>
         <v>-5.0060657805601608E-2</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="13">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
@@ -1946,7 +1950,7 @@
         <f t="shared" si="1"/>
         <v>-1.2912833886247806E-2</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="13">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
@@ -2005,7 +2009,7 @@
         <f t="shared" si="1"/>
         <v>-1.3637949218750009E-2</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="13">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
@@ -2064,7 +2068,7 @@
         <f t="shared" si="1"/>
         <v>3.1837408866824991E-3</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="13">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -2123,7 +2127,7 @@
         <f t="shared" si="1"/>
         <v>-1.1850188616360429E-2</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="13">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
@@ -2182,7 +2186,7 @@
         <f t="shared" si="1"/>
         <v>-2.8351094826658003E-2</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="13">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
@@ -2241,7 +2245,7 @@
         <f t="shared" si="1"/>
         <v>-5.4037002206391245E-2</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="13">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
@@ -2300,7 +2304,7 @@
         <f t="shared" si="1"/>
         <v>-4.258504294298146E-2</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="13">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
@@ -2359,7 +2363,7 @@
         <f t="shared" si="1"/>
         <v>-1.2379538203300809E-5</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="13">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
@@ -2418,7 +2422,7 @@
         <f t="shared" si="1"/>
         <v>-7.9052463618023094E-2</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="13">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
@@ -2477,7 +2481,7 @@
         <f t="shared" si="1"/>
         <v>-1.3285502334437123E-2</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="13">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
@@ -2536,7 +2540,7 @@
         <f t="shared" si="1"/>
         <v>-3.9590110100806722E-2</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
@@ -2595,7 +2599,7 @@
         <f t="shared" si="1"/>
         <v>-1.3334943305713101E-2</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="13">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
@@ -2654,7 +2658,7 @@
         <f t="shared" si="1"/>
         <v>-1.0226130964676661E-2</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="13">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
@@ -2713,7 +2717,7 @@
         <f t="shared" si="1"/>
         <v>-8.5306091660634673E-2</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="13">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
@@ -2772,7 +2776,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F27" s="17" t="str">
+      <c r="F27" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2831,7 +2835,7 @@
         <f t="shared" si="1"/>
         <v>-9.5782760864849215E-2</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="13">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
@@ -2890,7 +2894,7 @@
         <f t="shared" si="1"/>
         <v>-1.4800253727847622E-2</v>
       </c>
-      <c r="F29" s="17">
+      <c r="F29" s="13">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
@@ -2949,7 +2953,7 @@
         <f t="shared" si="1"/>
         <v>-8.3831374359143746E-3</v>
       </c>
-      <c r="F30" s="17">
+      <c r="F30" s="13">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
@@ -3008,7 +3012,7 @@
         <f t="shared" si="1"/>
         <v>-1.4030533529678329E-2</v>
       </c>
-      <c r="F31" s="17">
+      <c r="F31" s="13">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
@@ -3067,7 +3071,7 @@
         <f t="shared" si="1"/>
         <v>-1.2294942827617691E-2</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F32" s="13">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
@@ -3126,7 +3130,7 @@
         <f t="shared" si="1"/>
         <v>-7.9969930789269058E-3</v>
       </c>
-      <c r="F33" s="17">
+      <c r="F33" s="13">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -3185,7 +3189,7 @@
         <f t="shared" si="1"/>
         <v>-1.8939149738619768E-2</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F34" s="13">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
@@ -3244,7 +3248,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F35" s="17" t="str">
+      <c r="F35" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3303,7 +3307,7 @@
         <f t="shared" si="1"/>
         <v>-7.8647857679780775E-2</v>
       </c>
-      <c r="F36" s="17">
+      <c r="F36" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
@@ -3362,7 +3366,7 @@
         <f t="shared" si="1"/>
         <v>-3.9444515758219188E-2</v>
       </c>
-      <c r="F37" s="17">
+      <c r="F37" s="13">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
@@ -3421,7 +3425,7 @@
         <f t="shared" si="1"/>
         <v>-1.9443680579913542E-2</v>
       </c>
-      <c r="F38" s="17">
+      <c r="F38" s="13">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
@@ -3480,7 +3484,7 @@
         <f t="shared" si="1"/>
         <v>-8.008952370177623E-2</v>
       </c>
-      <c r="F39" s="17">
+      <c r="F39" s="13">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
@@ -3539,7 +3543,7 @@
         <f t="shared" si="1"/>
         <v>-2.1279773539092578E-2</v>
       </c>
-      <c r="F40" s="17">
+      <c r="F40" s="13">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
@@ -3598,7 +3602,7 @@
         <f t="shared" si="1"/>
         <v>-4.0110550149132493E-2</v>
       </c>
-      <c r="F41" s="17">
+      <c r="F41" s="13">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
@@ -3657,7 +3661,7 @@
         <f t="shared" si="1"/>
         <v>-2.2070943135841053E-4</v>
       </c>
-      <c r="F42" s="17">
+      <c r="F42" s="13">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -3716,7 +3720,7 @@
         <f t="shared" si="1"/>
         <v>-2.0497353541313264E-2</v>
       </c>
-      <c r="F43" s="17">
+      <c r="F43" s="13">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
@@ -3775,7 +3779,7 @@
         <f t="shared" si="1"/>
         <v>-9.7760750186150751E-3</v>
       </c>
-      <c r="F44" s="17">
+      <c r="F44" s="13">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -3834,7 +3838,7 @@
         <f t="shared" si="1"/>
         <v>-1.287514194887851E-2</v>
       </c>
-      <c r="F45" s="17">
+      <c r="F45" s="13">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
@@ -3893,7 +3897,7 @@
         <f t="shared" si="1"/>
         <v>-3.0010420686993711E-3</v>
       </c>
-      <c r="F46" s="17">
+      <c r="F46" s="13">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
@@ -3952,7 +3956,7 @@
         <f t="shared" si="1"/>
         <v>-1.7435939690898361E-4</v>
       </c>
-      <c r="F47" s="17">
+      <c r="F47" s="13">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
@@ -4011,7 +4015,7 @@
         <f t="shared" si="1"/>
         <v>-3.1133192323107857E-2</v>
       </c>
-      <c r="F48" s="17">
+      <c r="F48" s="13">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
@@ -4070,7 +4074,7 @@
         <f t="shared" si="1"/>
         <v>-1.8444360086767971E-2</v>
       </c>
-      <c r="F49" s="17">
+      <c r="F49" s="13">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
@@ -4129,7 +4133,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F50" s="17">
+      <c r="F50" s="13">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -4188,7 +4192,7 @@
         <f t="shared" si="1"/>
         <v>-1.2785255822058129E-2</v>
       </c>
-      <c r="F51" s="17">
+      <c r="F51" s="13">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
@@ -4247,7 +4251,7 @@
         <f t="shared" si="1"/>
         <v>-8.009596083231342E-2</v>
       </c>
-      <c r="F52" s="17">
+      <c r="F52" s="13">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
@@ -4306,7 +4310,7 @@
       <c r="D55" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E55" s="9" t="s">
+      <c r="E55" s="10" t="s">
         <v>90</v>
       </c>
       <c r="F55" s="14" t="s">
@@ -4338,20 +4342,20 @@
         <f>VLOOKUP($A56,$A$1:N$52,14,FALSE)</f>
         <v>-9181.0800000000163</v>
       </c>
-      <c r="E56" s="10"/>
+      <c r="E56" s="11"/>
       <c r="F56" s="13" t="s">
         <v>24</v>
       </c>
       <c r="G56">
-        <f>INDEX(D$2:D$52,MATCH($F56,$A$2:$A$52))</f>
+        <f t="shared" ref="G56:G61" si="9">INDEX(D$2:D$52,MATCH($F56,$A$2:$A$52))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="H56">
-        <f t="shared" ref="H56:I61" si="9">INDEX(E$2:E$52,MATCH($F56,$A$2:$A$52))</f>
+        <f t="shared" ref="H56:I61" si="10">INDEX(E$2:E$52,MATCH($F56,$A$2:$A$52))</f>
         <v>-8.1681998646514792E-2</v>
       </c>
       <c r="I56">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>43</v>
       </c>
     </row>
@@ -4360,31 +4364,31 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="10">VLOOKUP(A57,A$1:D$52,4,FALSE)</f>
+        <f t="shared" ref="B57:B61" si="11">VLOOKUP(A57,A$1:D$52,4,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:C61" si="11">VLOOKUP(A57,A$1:I$52,9,FALSE)</f>
+        <f t="shared" ref="C57:C61" si="12">VLOOKUP(A57,A$1:I$52,9,FALSE)</f>
         <v>0</v>
       </c>
       <c r="D57">
         <f>VLOOKUP($A57,$A$1:N$52,14,FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
-      <c r="E57" s="10"/>
+      <c r="E57" s="11"/>
       <c r="F57" s="13" t="s">
         <v>25</v>
       </c>
       <c r="G57">
-        <f t="shared" ref="G57:G61" si="12">INDEX(D$2:D$52,MATCH($F57,$A$2:$A$52))</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -4393,31 +4397,31 @@
         <v>32</v>
       </c>
       <c r="B58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
         <f>VLOOKUP($A58,$A$1:N$52,14,FALSE)</f>
         <v>-374962.91000000015</v>
       </c>
-      <c r="E58" s="10"/>
+      <c r="E58" s="11"/>
       <c r="F58" s="13" t="s">
         <v>32</v>
       </c>
       <c r="G58">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="H58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-5.4037002206391245E-2</v>
       </c>
       <c r="I58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>37</v>
       </c>
     </row>
@@ -4426,31 +4430,31 @@
         <v>38</v>
       </c>
       <c r="B59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
         <f>VLOOKUP($A59,$A$1:N$52,14,FALSE)</f>
         <v>-72.879999999888241</v>
       </c>
-      <c r="E59" s="10"/>
+      <c r="E59" s="11"/>
       <c r="F59" s="13" t="s">
         <v>38</v>
       </c>
       <c r="G59">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="H59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.3334943305713101E-2</v>
       </c>
       <c r="I59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>18</v>
       </c>
     </row>
@@ -4459,31 +4463,31 @@
         <v>39</v>
       </c>
       <c r="B60">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
         <f>VLOOKUP($A60,$A$1:N$52,14,FALSE)</f>
         <v>-1724.9000000000233</v>
       </c>
-      <c r="E60" s="10"/>
+      <c r="E60" s="11"/>
       <c r="F60" s="13" t="s">
         <v>39</v>
       </c>
       <c r="G60">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="H60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.0226130964676661E-2</v>
       </c>
       <c r="I60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
     </row>
@@ -4492,36 +4496,36 @@
         <v>55</v>
       </c>
       <c r="B61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
         <f>VLOOKUP($A61,$A$1:N$52,14,FALSE)</f>
         <v>-82077.349999999627</v>
       </c>
-      <c r="E61" s="10"/>
+      <c r="E61" s="11"/>
       <c r="F61" s="13" t="s">
         <v>55</v>
       </c>
       <c r="G61">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="H61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-4.0110550149132493E-2</v>
       </c>
       <c r="I61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:16">
-      <c r="E62" s="10"/>
+      <c r="E62" s="11"/>
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="7" t="s">
@@ -4879,7 +4883,7 @@
         <f>_xlfn.XLOOKUP(B$89,$F$1:$F$52,$A$1:$A$52)</f>
         <v>Debt Service</v>
       </c>
-      <c r="C91" s="12">
+      <c r="C91" s="9">
         <f>_xlfn.XLOOKUP(B91,$A$1:$A$52,$E$1:$E$52)</f>
         <v>3.1837408866824991E-3</v>
       </c>
@@ -4887,7 +4891,7 @@
         <f>_xlfn.XLOOKUP(D$89,$F$1:$F$52,$A$1:$A$52)</f>
         <v>Sports Authority</v>
       </c>
-      <c r="E91" s="12">
+      <c r="E91" s="9">
         <f>_xlfn.XLOOKUP(D91,$A$1:$A$52,$E$1:$E$52)</f>
         <v>0</v>
       </c>
@@ -4895,7 +4899,7 @@
         <f>_xlfn.XLOOKUP(F$89,$F$1:$F$52,$A$1:$A$52)</f>
         <v>Fire</v>
       </c>
-      <c r="G91" s="12">
+      <c r="G91" s="9">
         <f>_xlfn.XLOOKUP(F91,$A$1:$A$52,$E$1:$E$52)</f>
         <v>-1.2379538203300809E-5</v>
       </c>
@@ -4908,7 +4912,7 @@
         <f>_xlfn.XLOOKUP(B$89,$K$1:$K$52,$A$1:$A$52)</f>
         <v>Sports Authority</v>
       </c>
-      <c r="C92" s="12">
+      <c r="C92" s="9">
         <f>_xlfn.XLOOKUP(B92,$A$1:$A$52,$J$1:$J$52)</f>
         <v>0</v>
       </c>
@@ -4916,7 +4920,7 @@
         <f>_xlfn.XLOOKUP(D$89,$K$1:$K$52,$A$1:$A$52)</f>
         <v>Fire</v>
       </c>
-      <c r="E92" s="12">
+      <c r="E92" s="9">
         <f>_xlfn.XLOOKUP(D92,$A$1:$A$52,$J$1:$J$52)</f>
         <v>-7.4142392760188761E-5</v>
       </c>
@@ -4924,7 +4928,7 @@
         <f>_xlfn.XLOOKUP(F$89,$K$1:$K$52,$A$1:$A$52)</f>
         <v>District Attorney</v>
       </c>
-      <c r="G92" s="12">
+      <c r="G92" s="9">
         <f>_xlfn.XLOOKUP(F92,$A$1:$A$52,$J$1:$J$52)</f>
         <v>-2.769017341040361E-4</v>
       </c>
@@ -4937,7 +4941,7 @@
         <f>_xlfn.XLOOKUP(B$89,$P$1:$P$52,$A$1:$A$52)</f>
         <v>Sports Authority</v>
       </c>
-      <c r="C93" s="12">
+      <c r="C93" s="9">
         <f>_xlfn.XLOOKUP(B93,$A$1:$A$52,$O$1:$O$52)</f>
         <v>0</v>
       </c>
@@ -4945,7 +4949,7 @@
         <f>_xlfn.XLOOKUP(D$89,$P$1:$P$52,$A$1:$A$52)</f>
         <v>Police</v>
       </c>
-      <c r="E93" s="12">
+      <c r="E93" s="9">
         <f>_xlfn.XLOOKUP(D93,$A$1:$A$52,$O$1:$O$52)</f>
         <v>-1.8129115815929696E-7</v>
       </c>
@@ -4953,7 +4957,7 @@
         <f>_xlfn.XLOOKUP(F$89,$P$1:$P$52,$A$1:$A$52)</f>
         <v>Fire</v>
       </c>
-      <c r="G93" s="12">
+      <c r="G93" s="9">
         <f>_xlfn.XLOOKUP(F93,$A$1:$A$52,$O$1:$O$52)</f>
         <v>-8.9158438821450736E-7</v>
       </c>
@@ -4967,11 +4971,11 @@
       <c r="A96" t="s">
         <v>77</v>
       </c>
-      <c r="B96" s="7">
+      <c r="B96" s="17">
         <v>1</v>
       </c>
       <c r="C96" s="7"/>
-      <c r="D96" s="7">
+      <c r="D96" s="17">
         <v>2</v>
       </c>
       <c r="E96" s="7"/>
@@ -5003,54 +5007,132 @@
       <c r="A98" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="G98" s="4"/>
+      <c r="B98" t="str">
+        <f>INDEX(A1:A52,(MATCH(B96,F1:F52,0)))</f>
+        <v>Debt Service</v>
+      </c>
+      <c r="C98" s="9">
+        <f>INDEX($E$1:$E$52,MATCH(B$98,$A$1:$A$52))</f>
+        <v>3.1837408866824991E-3</v>
+      </c>
+      <c r="D98" t="str">
+        <f>INDEX($A$1:$A$52,MATCH(D$96,$F$1:$F$52,0))</f>
+        <v>Sports Authority</v>
+      </c>
+      <c r="E98" s="9">
+        <f>INDEX($E$1:$E$52,MATCH(D$98,$A$1:$A$52))</f>
+        <v>0</v>
+      </c>
+      <c r="F98" t="str">
+        <f>INDEX($A$1:$A$52,MATCH(F$96,$F$1:$F$52,0))</f>
+        <v>Fire</v>
+      </c>
+      <c r="G98" s="9">
+        <f>INDEX($E$1:$E$52,MATCH(F$98,$A$1:$A$52))</f>
+        <v>-1.2379538203300809E-5</v>
+      </c>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="G99" s="4"/>
+      <c r="B99" t="str">
+        <f>INDEX($A$1:$A$52,MATCH(B$96,$K$1:$K$52,0))</f>
+        <v>Sports Authority</v>
+      </c>
+      <c r="C99" s="9">
+        <f>INDEX($J$2:$J$52,MATCH(B$99,$A$2:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="D99" t="str">
+        <f>INDEX($A$1:$A$52,MATCH(D$96,$K$1:$K$52,0))</f>
+        <v>Fire</v>
+      </c>
+      <c r="E99" s="9">
+        <f>INDEX($J$2:$J$52,MATCH(D$99,$A$2:$A$52,0))</f>
+        <v>-7.4142392760188761E-5</v>
+      </c>
+      <c r="F99" t="str">
+        <f>INDEX($A$1:$A$52,MATCH(F$96,$K$1:$K$52,0))</f>
+        <v>District Attorney</v>
+      </c>
+      <c r="G99" s="9">
+        <f>INDEX($J$2:$J$52,MATCH(F$99,$A$2:$A$52,0))</f>
+        <v>-2.769017341040361E-4</v>
+      </c>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>75</v>
       </c>
-      <c r="C100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="G100" s="4"/>
+      <c r="B100" t="str">
+        <f>INDEX($A$2:$A$52,MATCH(B$96,$P$2:$P$52,0))</f>
+        <v>Sports Authority</v>
+      </c>
+      <c r="C100" s="9">
+        <f>INDEX($O$2:$O$52,MATCH(B$100,$A$2:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="D100" t="str">
+        <f>INDEX($A$2:$A$52,MATCH(D$96,$P$2:$P$52,0))</f>
+        <v>Police</v>
+      </c>
+      <c r="E100" s="18">
+        <f>INDEX($O$2:$O$52,MATCH(D$100,$A$2:$A$52,0))</f>
+        <v>-1.8129115815929696E-7</v>
+      </c>
+      <c r="F100" t="str">
+        <f>INDEX($A$2:$A$52,MATCH(F$96,$P$2:$P$52,0))</f>
+        <v>Fire</v>
+      </c>
+      <c r="G100" s="18">
+        <f>INDEX($O$2:$O$52,MATCH(F$100,$A$2:$A$52,0))</f>
+        <v>-8.9158438821450736E-7</v>
+      </c>
       <c r="I100" s="4"/>
     </row>
     <row r="103" spans="1:9">
-      <c r="A103" s="11" t="s">
+      <c r="A103" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B103" s="11"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
+      <c r="B103" s="12"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="12"/>
     </row>
     <row r="104" spans="1:9">
-      <c r="A104" s="11"/>
-      <c r="B104" s="11"/>
-      <c r="C104" s="11"/>
-      <c r="D104" s="11"/>
+      <c r="A104" s="12"/>
+      <c r="B104" s="12"/>
+      <c r="C104" s="12"/>
+      <c r="D104" s="12"/>
     </row>
     <row r="105" spans="1:9">
-      <c r="A105" s="11"/>
-      <c r="B105" s="11"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
+      <c r="A105" s="12"/>
+      <c r="B105" s="12"/>
+      <c r="C105" s="12"/>
+      <c r="D105" s="12"/>
+    </row>
+    <row r="107" spans="1:9" ht="14.5" customHeight="1">
+      <c r="A107" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B107" s="12"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" s="12"/>
+      <c r="B108" s="12"/>
+      <c r="C108" s="12"/>
+      <c r="D108" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:P52" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E55:E62"/>
     <mergeCell ref="A103:D105"/>
+    <mergeCell ref="A107:D108"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A82:A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
@@ -5059,6 +5141,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>